<commit_message>
CPU Microcode signals update
</commit_message>
<xml_diff>
--- a/Other/CPU MicroCode Signals.xlsx
+++ b/Other/CPU MicroCode Signals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Libraries\Documents\MAX7000CPU-GEN2\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1269EB-88D4-476F-B52D-B734E7DA67C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AB12D7-9E02-4861-AE88-E1906902D4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3061861A-EC9A-EA49-8D55-92F43BFE0D9E}"/>
   </bookViews>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA06146-33F3-F747-834E-F5D5B9EC84C7}">
   <dimension ref="A1:AD265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19599,7 +19599,7 @@
         <v>1</v>
       </c>
       <c r="T231">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U231">
         <v>1</v>
@@ -20426,7 +20426,7 @@
         <v>0</v>
       </c>
       <c r="O241">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P241">
         <v>0</v>

</xml_diff>